<commit_message>
Update excel with time measurements
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -51,9 +51,6 @@
     <t>Real time (ms)</t>
   </si>
   <si>
-    <t>20 valores desde 1 y por debajo de 10000000</t>
-  </si>
-  <si>
     <t>Intel Core i7-7500U 2.70 GHz - 2.90 GHz, 16GB RAM (2 núcleos, 2 hilos por núcleo)</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>Clase Problem001Parallel</t>
+  </si>
+  <si>
+    <t>20 valores: Múltiples de 3 o 5 desde 1 y por debajo de 10000000</t>
   </si>
 </sst>
 </file>
@@ -197,24 +197,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -531,29 +531,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -622,988 +622,31 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>1</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-      <c r="G5">
-        <v>6</v>
-      </c>
-      <c r="H5">
-        <v>7</v>
-      </c>
-      <c r="I5">
-        <v>6</v>
-      </c>
-      <c r="J5">
-        <v>7</v>
-      </c>
-      <c r="K5">
-        <v>5</v>
-      </c>
-      <c r="L5">
-        <v>6</v>
-      </c>
-      <c r="M5">
-        <v>7</v>
-      </c>
-      <c r="N5">
-        <v>7</v>
-      </c>
-      <c r="O5">
-        <v>8</v>
-      </c>
-      <c r="P5">
-        <v>7</v>
-      </c>
-      <c r="Q5">
-        <v>14</v>
-      </c>
-      <c r="R5">
-        <v>13</v>
-      </c>
-      <c r="S5">
-        <v>12</v>
-      </c>
-      <c r="T5">
-        <v>11</v>
-      </c>
-      <c r="U5" s="1">
-        <f>AVERAGE(A5:T5)</f>
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>346</v>
-      </c>
-      <c r="B8">
-        <v>337</v>
-      </c>
-      <c r="C8">
-        <v>332</v>
-      </c>
-      <c r="D8">
-        <v>334</v>
-      </c>
-      <c r="E8">
-        <v>334</v>
-      </c>
-      <c r="F8">
-        <v>336</v>
-      </c>
-      <c r="G8">
-        <v>336</v>
-      </c>
-      <c r="H8">
-        <v>338</v>
-      </c>
-      <c r="I8">
-        <v>336</v>
-      </c>
-      <c r="J8">
-        <v>337</v>
-      </c>
-      <c r="K8">
-        <v>346</v>
-      </c>
-      <c r="L8">
-        <v>350</v>
-      </c>
-      <c r="M8">
-        <v>343</v>
-      </c>
-      <c r="N8">
-        <v>338</v>
-      </c>
-      <c r="O8">
-        <v>352</v>
-      </c>
-      <c r="P8">
-        <v>341</v>
-      </c>
-      <c r="Q8">
-        <v>351</v>
-      </c>
-      <c r="R8">
-        <v>341</v>
-      </c>
-      <c r="S8">
-        <v>336</v>
-      </c>
-      <c r="T8">
-        <v>343</v>
-      </c>
-      <c r="U8" s="1">
-        <f>AVERAGE(A8:T8)</f>
-        <v>340.35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>3796</v>
-      </c>
-      <c r="B11">
-        <v>3776</v>
-      </c>
-      <c r="C11">
-        <v>3771</v>
-      </c>
-      <c r="D11">
-        <v>3789</v>
-      </c>
-      <c r="E11">
-        <v>3981</v>
-      </c>
-      <c r="F11">
-        <v>3808</v>
-      </c>
-      <c r="G11">
-        <v>3808</v>
-      </c>
-      <c r="H11">
-        <v>3830</v>
-      </c>
-      <c r="I11">
-        <v>3786</v>
-      </c>
-      <c r="J11">
-        <v>3785</v>
-      </c>
-      <c r="K11">
-        <v>3796</v>
-      </c>
-      <c r="L11">
-        <v>3791</v>
-      </c>
-      <c r="M11">
-        <v>3924</v>
-      </c>
-      <c r="N11">
-        <v>3814</v>
-      </c>
-      <c r="O11">
-        <v>3802</v>
-      </c>
-      <c r="P11">
-        <v>3792</v>
-      </c>
-      <c r="Q11">
-        <v>3813</v>
-      </c>
-      <c r="R11">
-        <v>3817</v>
-      </c>
-      <c r="S11">
-        <v>3807</v>
-      </c>
-      <c r="T11">
-        <v>3782</v>
-      </c>
-      <c r="U11" s="1">
-        <f>AVERAGE(A11:T11)</f>
-        <v>3813.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>4201</v>
-      </c>
-      <c r="B14">
-        <v>4170</v>
-      </c>
-      <c r="C14">
-        <v>4154</v>
-      </c>
-      <c r="D14">
-        <v>4185</v>
-      </c>
-      <c r="E14">
-        <v>4171</v>
-      </c>
-      <c r="F14">
-        <v>4173</v>
-      </c>
-      <c r="G14">
-        <v>4569</v>
-      </c>
-      <c r="H14">
-        <v>4288</v>
-      </c>
-      <c r="I14">
-        <v>4165</v>
-      </c>
-      <c r="J14">
-        <v>4155</v>
-      </c>
-      <c r="K14">
-        <v>4143</v>
-      </c>
-      <c r="L14">
-        <v>4167</v>
-      </c>
-      <c r="M14">
-        <v>4154</v>
-      </c>
-      <c r="N14">
-        <v>4174</v>
-      </c>
-      <c r="O14">
-        <v>4205</v>
-      </c>
-      <c r="P14">
-        <v>4220</v>
-      </c>
-      <c r="Q14">
-        <v>4158</v>
-      </c>
-      <c r="R14">
-        <v>4143</v>
-      </c>
-      <c r="S14">
-        <v>4396</v>
-      </c>
-      <c r="T14">
-        <v>4153</v>
-      </c>
-      <c r="U14" s="1">
-        <f>AVERAGE(A14:T14)</f>
-        <v>4207.2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>395</v>
-      </c>
-      <c r="B17">
-        <v>384</v>
-      </c>
-      <c r="C17">
-        <v>384</v>
-      </c>
-      <c r="D17">
-        <v>403</v>
-      </c>
-      <c r="E17">
-        <v>390</v>
-      </c>
-      <c r="F17">
-        <v>399</v>
-      </c>
-      <c r="G17">
-        <v>387</v>
-      </c>
-      <c r="H17">
-        <v>383</v>
-      </c>
-      <c r="I17">
-        <v>391</v>
-      </c>
-      <c r="J17">
-        <v>396</v>
-      </c>
-      <c r="K17">
-        <v>386</v>
-      </c>
-      <c r="L17">
-        <v>388</v>
-      </c>
-      <c r="M17">
-        <v>393</v>
-      </c>
-      <c r="N17">
-        <v>386</v>
-      </c>
-      <c r="O17">
-        <v>389</v>
-      </c>
-      <c r="P17">
-        <v>388</v>
-      </c>
-      <c r="Q17">
-        <v>388</v>
-      </c>
-      <c r="R17">
-        <v>399</v>
-      </c>
-      <c r="S17">
-        <v>384</v>
-      </c>
-      <c r="T17">
-        <v>393</v>
-      </c>
-      <c r="U17" s="1">
-        <f>AVERAGE(A17:T17)</f>
-        <v>390.3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>6352</v>
-      </c>
-      <c r="B20">
-        <v>6412</v>
-      </c>
-      <c r="C20">
-        <v>6342</v>
-      </c>
-      <c r="D20">
-        <v>6347</v>
-      </c>
-      <c r="E20">
-        <v>6326</v>
-      </c>
-      <c r="F20">
-        <v>6339</v>
-      </c>
-      <c r="G20">
-        <v>6330</v>
-      </c>
-      <c r="H20">
-        <v>6337</v>
-      </c>
-      <c r="I20">
-        <v>6335</v>
-      </c>
-      <c r="J20">
-        <v>6345</v>
-      </c>
-      <c r="K20">
-        <v>6346</v>
-      </c>
-      <c r="L20">
-        <v>6340</v>
-      </c>
-      <c r="M20">
-        <v>6332</v>
-      </c>
-      <c r="N20">
-        <v>6301</v>
-      </c>
-      <c r="O20">
-        <v>6349</v>
-      </c>
-      <c r="P20">
-        <v>6339</v>
-      </c>
-      <c r="Q20">
-        <v>6554</v>
-      </c>
-      <c r="R20">
-        <v>6360</v>
-      </c>
-      <c r="S20">
-        <v>6344</v>
-      </c>
-      <c r="T20">
-        <v>6354</v>
-      </c>
-      <c r="U20" s="1">
-        <f>AVERAGE(A20:T20)</f>
-        <v>6354.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2293</v>
-      </c>
-      <c r="B23">
-        <v>2279</v>
-      </c>
-      <c r="C23">
-        <v>2283</v>
-      </c>
-      <c r="D23">
-        <v>2303</v>
-      </c>
-      <c r="E23">
-        <v>2290</v>
-      </c>
-      <c r="F23">
-        <v>2296</v>
-      </c>
-      <c r="G23">
-        <v>2270</v>
-      </c>
-      <c r="H23">
-        <v>2290</v>
-      </c>
-      <c r="I23">
-        <v>2284</v>
-      </c>
-      <c r="J23">
-        <v>2286</v>
-      </c>
-      <c r="K23">
-        <v>2281</v>
-      </c>
-      <c r="L23">
-        <v>2271</v>
-      </c>
-      <c r="M23">
-        <v>2286</v>
-      </c>
-      <c r="N23">
-        <v>2276</v>
-      </c>
-      <c r="O23">
-        <v>2290</v>
-      </c>
-      <c r="P23">
-        <v>2261</v>
-      </c>
-      <c r="Q23">
-        <v>2287</v>
-      </c>
-      <c r="R23">
-        <v>2273</v>
-      </c>
-      <c r="S23">
-        <v>2272</v>
-      </c>
-      <c r="T23">
-        <v>2291</v>
-      </c>
-      <c r="U23" s="1">
-        <f>AVERAGE(A23:T23)</f>
-        <v>2283.1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>834</v>
-      </c>
-      <c r="B26">
-        <v>830</v>
-      </c>
-      <c r="C26">
-        <v>827</v>
-      </c>
-      <c r="D26">
-        <v>828</v>
-      </c>
-      <c r="E26">
-        <v>826</v>
-      </c>
-      <c r="F26">
-        <v>825</v>
-      </c>
-      <c r="G26">
-        <v>824</v>
-      </c>
-      <c r="H26">
-        <v>822</v>
-      </c>
-      <c r="I26">
-        <v>828</v>
-      </c>
-      <c r="J26">
-        <v>833</v>
-      </c>
-      <c r="K26">
-        <v>824</v>
-      </c>
-      <c r="L26">
-        <v>828</v>
-      </c>
-      <c r="M26">
-        <v>832</v>
-      </c>
-      <c r="N26">
-        <v>831</v>
-      </c>
-      <c r="O26">
-        <v>834</v>
-      </c>
-      <c r="P26">
-        <v>818</v>
-      </c>
-      <c r="Q26">
-        <v>818</v>
-      </c>
-      <c r="R26">
-        <v>830</v>
-      </c>
-      <c r="S26">
-        <v>835</v>
-      </c>
-      <c r="T26">
-        <v>833</v>
-      </c>
-      <c r="U26" s="1">
-        <f>AVERAGE(A26:T26)</f>
-        <v>828</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A12:U12"/>
-    <mergeCell ref="A13:U13"/>
-    <mergeCell ref="A15:U15"/>
-    <mergeCell ref="A16:U16"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A4:U4"/>
-    <mergeCell ref="A7:U7"/>
-    <mergeCell ref="A3:U3"/>
-    <mergeCell ref="A6:U6"/>
-    <mergeCell ref="A10:U10"/>
-    <mergeCell ref="A19:U19"/>
-    <mergeCell ref="A21:U21"/>
-    <mergeCell ref="A22:U22"/>
-    <mergeCell ref="A24:U24"/>
-    <mergeCell ref="A25:U25"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V54"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:V3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="21" width="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-    </row>
-    <row r="2" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-    </row>
-    <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1625,36 +668,993 @@
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <v>7</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>6</v>
+      </c>
+      <c r="M5">
+        <v>7</v>
+      </c>
+      <c r="N5">
+        <v>7</v>
+      </c>
+      <c r="O5">
+        <v>8</v>
+      </c>
+      <c r="P5">
+        <v>7</v>
+      </c>
+      <c r="Q5">
+        <v>14</v>
+      </c>
+      <c r="R5">
+        <v>13</v>
+      </c>
+      <c r="S5">
+        <v>12</v>
+      </c>
+      <c r="T5">
+        <v>11</v>
+      </c>
+      <c r="U5" s="1">
+        <f>AVERAGE(A5:T5)</f>
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>346</v>
+      </c>
+      <c r="B8">
+        <v>337</v>
+      </c>
+      <c r="C8">
+        <v>332</v>
+      </c>
+      <c r="D8">
+        <v>334</v>
+      </c>
+      <c r="E8">
+        <v>334</v>
+      </c>
+      <c r="F8">
+        <v>336</v>
+      </c>
+      <c r="G8">
+        <v>336</v>
+      </c>
+      <c r="H8">
+        <v>338</v>
+      </c>
+      <c r="I8">
+        <v>336</v>
+      </c>
+      <c r="J8">
+        <v>337</v>
+      </c>
+      <c r="K8">
+        <v>346</v>
+      </c>
+      <c r="L8">
+        <v>350</v>
+      </c>
+      <c r="M8">
+        <v>343</v>
+      </c>
+      <c r="N8">
+        <v>338</v>
+      </c>
+      <c r="O8">
+        <v>352</v>
+      </c>
+      <c r="P8">
+        <v>341</v>
+      </c>
+      <c r="Q8">
+        <v>351</v>
+      </c>
+      <c r="R8">
+        <v>341</v>
+      </c>
+      <c r="S8">
+        <v>336</v>
+      </c>
+      <c r="T8">
+        <v>343</v>
+      </c>
+      <c r="U8" s="1">
+        <f>AVERAGE(A8:T8)</f>
+        <v>340.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3796</v>
+      </c>
+      <c r="B11">
+        <v>3776</v>
+      </c>
+      <c r="C11">
+        <v>3771</v>
+      </c>
+      <c r="D11">
+        <v>3789</v>
+      </c>
+      <c r="E11">
+        <v>3981</v>
+      </c>
+      <c r="F11">
+        <v>3808</v>
+      </c>
+      <c r="G11">
+        <v>3808</v>
+      </c>
+      <c r="H11">
+        <v>3830</v>
+      </c>
+      <c r="I11">
+        <v>3786</v>
+      </c>
+      <c r="J11">
+        <v>3785</v>
+      </c>
+      <c r="K11">
+        <v>3796</v>
+      </c>
+      <c r="L11">
+        <v>3791</v>
+      </c>
+      <c r="M11">
+        <v>3924</v>
+      </c>
+      <c r="N11">
+        <v>3814</v>
+      </c>
+      <c r="O11">
+        <v>3802</v>
+      </c>
+      <c r="P11">
+        <v>3792</v>
+      </c>
+      <c r="Q11">
+        <v>3813</v>
+      </c>
+      <c r="R11">
+        <v>3817</v>
+      </c>
+      <c r="S11">
+        <v>3807</v>
+      </c>
+      <c r="T11">
+        <v>3782</v>
+      </c>
+      <c r="U11" s="1">
+        <f>AVERAGE(A11:T11)</f>
+        <v>3813.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4201</v>
+      </c>
+      <c r="B14">
+        <v>4170</v>
+      </c>
+      <c r="C14">
+        <v>4154</v>
+      </c>
+      <c r="D14">
+        <v>4185</v>
+      </c>
+      <c r="E14">
+        <v>4171</v>
+      </c>
+      <c r="F14">
+        <v>4173</v>
+      </c>
+      <c r="G14">
+        <v>4569</v>
+      </c>
+      <c r="H14">
+        <v>4288</v>
+      </c>
+      <c r="I14">
+        <v>4165</v>
+      </c>
+      <c r="J14">
+        <v>4155</v>
+      </c>
+      <c r="K14">
+        <v>4143</v>
+      </c>
+      <c r="L14">
+        <v>4167</v>
+      </c>
+      <c r="M14">
+        <v>4154</v>
+      </c>
+      <c r="N14">
+        <v>4174</v>
+      </c>
+      <c r="O14">
+        <v>4205</v>
+      </c>
+      <c r="P14">
+        <v>4220</v>
+      </c>
+      <c r="Q14">
+        <v>4158</v>
+      </c>
+      <c r="R14">
+        <v>4143</v>
+      </c>
+      <c r="S14">
+        <v>4396</v>
+      </c>
+      <c r="T14">
+        <v>4153</v>
+      </c>
+      <c r="U14" s="1">
+        <f>AVERAGE(A14:T14)</f>
+        <v>4207.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>395</v>
+      </c>
+      <c r="B17">
+        <v>384</v>
+      </c>
+      <c r="C17">
+        <v>384</v>
+      </c>
+      <c r="D17">
+        <v>403</v>
+      </c>
+      <c r="E17">
+        <v>390</v>
+      </c>
+      <c r="F17">
+        <v>399</v>
+      </c>
+      <c r="G17">
+        <v>387</v>
+      </c>
+      <c r="H17">
+        <v>383</v>
+      </c>
+      <c r="I17">
+        <v>391</v>
+      </c>
+      <c r="J17">
+        <v>396</v>
+      </c>
+      <c r="K17">
+        <v>386</v>
+      </c>
+      <c r="L17">
+        <v>388</v>
+      </c>
+      <c r="M17">
+        <v>393</v>
+      </c>
+      <c r="N17">
+        <v>386</v>
+      </c>
+      <c r="O17">
+        <v>389</v>
+      </c>
+      <c r="P17">
+        <v>388</v>
+      </c>
+      <c r="Q17">
+        <v>388</v>
+      </c>
+      <c r="R17">
+        <v>399</v>
+      </c>
+      <c r="S17">
+        <v>384</v>
+      </c>
+      <c r="T17">
+        <v>393</v>
+      </c>
+      <c r="U17" s="1">
+        <f>AVERAGE(A17:T17)</f>
+        <v>390.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>6352</v>
+      </c>
+      <c r="B20">
+        <v>6412</v>
+      </c>
+      <c r="C20">
+        <v>6342</v>
+      </c>
+      <c r="D20">
+        <v>6347</v>
+      </c>
+      <c r="E20">
+        <v>6326</v>
+      </c>
+      <c r="F20">
+        <v>6339</v>
+      </c>
+      <c r="G20">
+        <v>6330</v>
+      </c>
+      <c r="H20">
+        <v>6337</v>
+      </c>
+      <c r="I20">
+        <v>6335</v>
+      </c>
+      <c r="J20">
+        <v>6345</v>
+      </c>
+      <c r="K20">
+        <v>6346</v>
+      </c>
+      <c r="L20">
+        <v>6340</v>
+      </c>
+      <c r="M20">
+        <v>6332</v>
+      </c>
+      <c r="N20">
+        <v>6301</v>
+      </c>
+      <c r="O20">
+        <v>6349</v>
+      </c>
+      <c r="P20">
+        <v>6339</v>
+      </c>
+      <c r="Q20">
+        <v>6554</v>
+      </c>
+      <c r="R20">
+        <v>6360</v>
+      </c>
+      <c r="S20">
+        <v>6344</v>
+      </c>
+      <c r="T20">
+        <v>6354</v>
+      </c>
+      <c r="U20" s="1">
+        <f>AVERAGE(A20:T20)</f>
+        <v>6354.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2293</v>
+      </c>
+      <c r="B23">
+        <v>2279</v>
+      </c>
+      <c r="C23">
+        <v>2283</v>
+      </c>
+      <c r="D23">
+        <v>2303</v>
+      </c>
+      <c r="E23">
+        <v>2290</v>
+      </c>
+      <c r="F23">
+        <v>2296</v>
+      </c>
+      <c r="G23">
+        <v>2270</v>
+      </c>
+      <c r="H23">
+        <v>2290</v>
+      </c>
+      <c r="I23">
+        <v>2284</v>
+      </c>
+      <c r="J23">
+        <v>2286</v>
+      </c>
+      <c r="K23">
+        <v>2281</v>
+      </c>
+      <c r="L23">
+        <v>2271</v>
+      </c>
+      <c r="M23">
+        <v>2286</v>
+      </c>
+      <c r="N23">
+        <v>2276</v>
+      </c>
+      <c r="O23">
+        <v>2290</v>
+      </c>
+      <c r="P23">
+        <v>2261</v>
+      </c>
+      <c r="Q23">
+        <v>2287</v>
+      </c>
+      <c r="R23">
+        <v>2273</v>
+      </c>
+      <c r="S23">
+        <v>2272</v>
+      </c>
+      <c r="T23">
+        <v>2291</v>
+      </c>
+      <c r="U23" s="1">
+        <f>AVERAGE(A23:T23)</f>
+        <v>2283.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>834</v>
+      </c>
+      <c r="B26">
+        <v>830</v>
+      </c>
+      <c r="C26">
+        <v>827</v>
+      </c>
+      <c r="D26">
+        <v>828</v>
+      </c>
+      <c r="E26">
+        <v>826</v>
+      </c>
+      <c r="F26">
+        <v>825</v>
+      </c>
+      <c r="G26">
+        <v>824</v>
+      </c>
+      <c r="H26">
+        <v>822</v>
+      </c>
+      <c r="I26">
+        <v>828</v>
+      </c>
+      <c r="J26">
+        <v>833</v>
+      </c>
+      <c r="K26">
+        <v>824</v>
+      </c>
+      <c r="L26">
+        <v>828</v>
+      </c>
+      <c r="M26">
+        <v>832</v>
+      </c>
+      <c r="N26">
+        <v>831</v>
+      </c>
+      <c r="O26">
+        <v>834</v>
+      </c>
+      <c r="P26">
+        <v>818</v>
+      </c>
+      <c r="Q26">
+        <v>818</v>
+      </c>
+      <c r="R26">
+        <v>830</v>
+      </c>
+      <c r="S26">
+        <v>835</v>
+      </c>
+      <c r="T26">
+        <v>833</v>
+      </c>
+      <c r="U26" s="1">
+        <f>AVERAGE(A26:T26)</f>
+        <v>828</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A19:U19"/>
+    <mergeCell ref="A21:U21"/>
+    <mergeCell ref="A22:U22"/>
+    <mergeCell ref="A24:U24"/>
+    <mergeCell ref="A25:U25"/>
+    <mergeCell ref="A12:U12"/>
+    <mergeCell ref="A13:U13"/>
+    <mergeCell ref="A15:U15"/>
+    <mergeCell ref="A16:U16"/>
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A4:U4"/>
+    <mergeCell ref="A7:U7"/>
+    <mergeCell ref="A3:U3"/>
+    <mergeCell ref="A6:U6"/>
+    <mergeCell ref="A10:U10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:V1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="21" width="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+    </row>
+    <row r="2" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
       <c r="V4" s="2"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
       <c r="V5" s="2"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B6">
@@ -1723,7 +1723,7 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B7">
@@ -1786,39 +1786,39 @@
       <c r="U7">
         <v>1782</v>
       </c>
-      <c r="V7" s="5">
+      <c r="V7" s="3">
         <f>AVERAGE(B7:U7)</f>
         <v>1808.45</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
       <c r="V8" s="2"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B9">
@@ -1887,7 +1887,7 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B10">
@@ -1956,33 +1956,33 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
+      <c r="A11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
       <c r="V11" s="2"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B12">
@@ -2051,7 +2051,7 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B13">
@@ -2114,69 +2114,69 @@
       <c r="U13">
         <v>101</v>
       </c>
-      <c r="V13" s="5">
+      <c r="V13" s="3">
         <f>AVERAGE(B13:U13)</f>
         <v>100.45</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="V14" s="5"/>
+      <c r="V14" s="3"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="6"/>
+      <c r="A15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
       <c r="V15" s="2"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
+      <c r="A16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
       <c r="V16" s="2"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -2201,7 +2201,7 @@
       <c r="V17" s="2"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B18">
@@ -2270,7 +2270,7 @@
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B19">
@@ -2333,14 +2333,14 @@
       <c r="U19">
         <v>2111</v>
       </c>
-      <c r="V19" s="5">
+      <c r="V19" s="3">
         <f>AVERAGE(B19:U19)</f>
         <v>1939.85</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -2365,7 +2365,7 @@
       <c r="V20" s="2"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B21">
@@ -2428,13 +2428,13 @@
       <c r="U21">
         <v>1013</v>
       </c>
-      <c r="V21" s="5">
+      <c r="V21" s="3">
         <f>AVERAGE(B21:U21)</f>
         <v>865.55</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B22">
@@ -2504,7 +2504,7 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -2529,7 +2529,7 @@
       <c r="V23" s="2"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B24">
@@ -2592,13 +2592,13 @@
       <c r="U24">
         <v>672</v>
       </c>
-      <c r="V24" s="5">
+      <c r="V24" s="3">
         <f>AVERAGE(B24:U24)</f>
         <v>704.15</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B25">
@@ -2668,7 +2668,7 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -2693,7 +2693,7 @@
       <c r="V26" s="2"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B27">
@@ -2756,13 +2756,13 @@
       <c r="U27">
         <v>692</v>
       </c>
-      <c r="V27" s="5">
+      <c r="V27" s="3">
         <f>AVERAGE(B27:U27)</f>
         <v>693.35</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B28">
@@ -2831,34 +2831,34 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
+      <c r="A29" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
       <c r="V29" s="2"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -2883,7 +2883,7 @@
       <c r="V30" s="2"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B31">
@@ -2946,13 +2946,13 @@
       <c r="U31">
         <v>412</v>
       </c>
-      <c r="V31" s="5">
+      <c r="V31" s="3">
         <f>AVERAGE(B31:U31)</f>
         <v>414.55</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B32">
@@ -3015,14 +3015,14 @@
       <c r="U32">
         <v>1105</v>
       </c>
-      <c r="V32" s="5">
+      <c r="V32" s="3">
         <f>AVERAGE(B32:U32)</f>
         <v>1086.1500000000001</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -3047,7 +3047,7 @@
       <c r="V33" s="2"/>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B34">
@@ -3110,13 +3110,13 @@
       <c r="U34">
         <v>274</v>
       </c>
-      <c r="V34" s="5">
+      <c r="V34" s="3">
         <f>AVERAGE(B34:U34)</f>
         <v>270.45</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B35">
@@ -3186,7 +3186,7 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -3211,7 +3211,7 @@
       <c r="V36" s="2"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B37">
@@ -3280,7 +3280,7 @@
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B38">
@@ -3350,7 +3350,7 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -3375,7 +3375,7 @@
       <c r="V39" s="2"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B40">
@@ -3438,13 +3438,13 @@
       <c r="U40">
         <v>211</v>
       </c>
-      <c r="V40" s="5">
+      <c r="V40" s="3">
         <f>AVERAGE(B40:U40)</f>
         <v>214.75</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B41">
@@ -3507,40 +3507,40 @@
       <c r="U41">
         <v>614</v>
       </c>
-      <c r="V41" s="5">
+      <c r="V41" s="3">
         <f>AVERAGE(B41:U41)</f>
         <v>607.35</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
+      <c r="A42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="6"/>
+      <c r="R42" s="6"/>
+      <c r="S42" s="6"/>
+      <c r="T42" s="6"/>
+      <c r="U42" s="6"/>
       <c r="V42" s="2"/>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -3565,7 +3565,7 @@
       <c r="V43" s="2"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B44">
@@ -3634,7 +3634,7 @@
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B45">
@@ -3697,14 +3697,14 @@
       <c r="U45">
         <v>302</v>
       </c>
-      <c r="V45" s="5">
+      <c r="V45" s="3">
         <f>AVERAGE(B45:U45)</f>
         <v>301.55</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -3726,10 +3726,10 @@
       <c r="S46" s="7"/>
       <c r="T46" s="7"/>
       <c r="U46" s="7"/>
-      <c r="V46" s="5"/>
+      <c r="V46" s="3"/>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B47">
@@ -3798,7 +3798,7 @@
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B48">
@@ -3861,14 +3861,14 @@
       <c r="U48">
         <v>301</v>
       </c>
-      <c r="V48" s="5">
+      <c r="V48" s="3">
         <f>AVERAGE(B48:U48)</f>
         <v>300.95</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -3890,10 +3890,10 @@
       <c r="S49" s="7"/>
       <c r="T49" s="7"/>
       <c r="U49" s="7"/>
-      <c r="V49" s="5"/>
+      <c r="V49" s="3"/>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B50">
@@ -3962,7 +3962,7 @@
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B51">
@@ -4032,7 +4032,7 @@
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -4054,10 +4054,10 @@
       <c r="S52" s="7"/>
       <c r="T52" s="7"/>
       <c r="U52" s="7"/>
-      <c r="V52" s="5"/>
+      <c r="V52" s="3"/>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B53">
@@ -4126,7 +4126,7 @@
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B54">
@@ -4196,6 +4196,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A5:U5"/>
+    <mergeCell ref="A15:U15"/>
+    <mergeCell ref="A16:U16"/>
+    <mergeCell ref="A17:U17"/>
+    <mergeCell ref="A20:U20"/>
+    <mergeCell ref="A8:U8"/>
+    <mergeCell ref="A11:U11"/>
     <mergeCell ref="A46:U46"/>
     <mergeCell ref="A49:U49"/>
     <mergeCell ref="A52:U52"/>
@@ -4212,13 +4219,6 @@
     <mergeCell ref="A36:U36"/>
     <mergeCell ref="A39:U39"/>
     <mergeCell ref="A4:U4"/>
-    <mergeCell ref="A5:U5"/>
-    <mergeCell ref="A15:U15"/>
-    <mergeCell ref="A16:U16"/>
-    <mergeCell ref="A17:U17"/>
-    <mergeCell ref="A20:U20"/>
-    <mergeCell ref="A8:U8"/>
-    <mergeCell ref="A11:U11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactor of statistics. Upgrade measurements excel
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -199,10 +199,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -212,9 +215,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -531,29 +531,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -622,52 +622,52 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -736,52 +736,52 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -850,29 +850,29 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -941,52 +941,52 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1055,52 +1055,52 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="6"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -1169,29 +1169,29 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1260,52 +1260,52 @@
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6"/>
-      <c r="U22" s="6"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1374,52 +1374,52 @@
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
-      <c r="T25" s="6"/>
-      <c r="U25" s="6"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1489,11 +1489,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A19:U19"/>
-    <mergeCell ref="A21:U21"/>
-    <mergeCell ref="A22:U22"/>
-    <mergeCell ref="A24:U24"/>
-    <mergeCell ref="A25:U25"/>
     <mergeCell ref="A12:U12"/>
     <mergeCell ref="A13:U13"/>
     <mergeCell ref="A15:U15"/>
@@ -1504,6 +1499,11 @@
     <mergeCell ref="A3:U3"/>
     <mergeCell ref="A6:U6"/>
     <mergeCell ref="A10:U10"/>
+    <mergeCell ref="A19:U19"/>
+    <mergeCell ref="A21:U21"/>
+    <mergeCell ref="A22:U22"/>
+    <mergeCell ref="A24:U24"/>
+    <mergeCell ref="A25:U25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1515,142 +1515,142 @@
   <dimension ref="A1:V54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:V1"/>
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="21" width="5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
       <c r="V4" s="2"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
       <c r="V5" s="2"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -1792,29 +1792,29 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
       <c r="V8" s="2"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1956,29 +1956,29 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
       <c r="V11" s="2"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -2123,81 +2123,81 @@
       <c r="V14" s="3"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
       <c r="V15" s="2"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="6"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
       <c r="V16" s="2"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
       <c r="V17" s="2"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
@@ -2339,29 +2339,29 @@
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
       <c r="V20" s="2"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
@@ -2503,29 +2503,29 @@
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7"/>
-      <c r="U23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
       <c r="V23" s="2"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
@@ -2667,29 +2667,29 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="7"/>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="7"/>
-      <c r="S26" s="7"/>
-      <c r="T26" s="7"/>
-      <c r="U26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
       <c r="V26" s="2"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
@@ -2831,55 +2831,55 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="6"/>
-      <c r="U29" s="6"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
       <c r="V29" s="2"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="7"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-      <c r="S30" s="7"/>
-      <c r="T30" s="7"/>
-      <c r="U30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
+      <c r="U30" s="8"/>
       <c r="V30" s="2"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
@@ -3021,29 +3021,29 @@
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="7"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="7"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="8"/>
+      <c r="U33" s="8"/>
       <c r="V33" s="2"/>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
@@ -3185,29 +3185,29 @@
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7"/>
-      <c r="P36" s="7"/>
-      <c r="Q36" s="7"/>
-      <c r="R36" s="7"/>
-      <c r="S36" s="7"/>
-      <c r="T36" s="7"/>
-      <c r="U36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
       <c r="V36" s="2"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
@@ -3349,29 +3349,29 @@
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
-      <c r="O39" s="7"/>
-      <c r="P39" s="7"/>
-      <c r="Q39" s="7"/>
-      <c r="R39" s="7"/>
-      <c r="S39" s="7"/>
-      <c r="T39" s="7"/>
-      <c r="U39" s="7"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+      <c r="U39" s="8"/>
       <c r="V39" s="2"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
@@ -3513,55 +3513,55 @@
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="6"/>
-      <c r="S42" s="6"/>
-      <c r="T42" s="6"/>
-      <c r="U42" s="6"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="5"/>
+      <c r="U42" s="5"/>
       <c r="V42" s="2"/>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="7"/>
-      <c r="O43" s="7"/>
-      <c r="P43" s="7"/>
-      <c r="Q43" s="7"/>
-      <c r="R43" s="7"/>
-      <c r="S43" s="7"/>
-      <c r="T43" s="7"/>
-      <c r="U43" s="7"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+      <c r="T43" s="8"/>
+      <c r="U43" s="8"/>
       <c r="V43" s="2"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
@@ -3703,29 +3703,29 @@
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="7"/>
-      <c r="P46" s="7"/>
-      <c r="Q46" s="7"/>
-      <c r="R46" s="7"/>
-      <c r="S46" s="7"/>
-      <c r="T46" s="7"/>
-      <c r="U46" s="7"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8"/>
+      <c r="R46" s="8"/>
+      <c r="S46" s="8"/>
+      <c r="T46" s="8"/>
+      <c r="U46" s="8"/>
       <c r="V46" s="3"/>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
@@ -3867,29 +3867,29 @@
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="7"/>
-      <c r="M49" s="7"/>
-      <c r="N49" s="7"/>
-      <c r="O49" s="7"/>
-      <c r="P49" s="7"/>
-      <c r="Q49" s="7"/>
-      <c r="R49" s="7"/>
-      <c r="S49" s="7"/>
-      <c r="T49" s="7"/>
-      <c r="U49" s="7"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8"/>
+      <c r="R49" s="8"/>
+      <c r="S49" s="8"/>
+      <c r="T49" s="8"/>
+      <c r="U49" s="8"/>
       <c r="V49" s="3"/>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
@@ -4031,29 +4031,29 @@
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="7"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="7"/>
-      <c r="O52" s="7"/>
-      <c r="P52" s="7"/>
-      <c r="Q52" s="7"/>
-      <c r="R52" s="7"/>
-      <c r="S52" s="7"/>
-      <c r="T52" s="7"/>
-      <c r="U52" s="7"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8"/>
+      <c r="O52" s="8"/>
+      <c r="P52" s="8"/>
+      <c r="Q52" s="8"/>
+      <c r="R52" s="8"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="8"/>
+      <c r="U52" s="8"/>
       <c r="V52" s="3"/>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
@@ -4196,13 +4196,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A5:U5"/>
-    <mergeCell ref="A15:U15"/>
-    <mergeCell ref="A16:U16"/>
-    <mergeCell ref="A17:U17"/>
-    <mergeCell ref="A20:U20"/>
-    <mergeCell ref="A8:U8"/>
-    <mergeCell ref="A11:U11"/>
     <mergeCell ref="A46:U46"/>
     <mergeCell ref="A49:U49"/>
     <mergeCell ref="A52:U52"/>
@@ -4219,6 +4212,13 @@
     <mergeCell ref="A36:U36"/>
     <mergeCell ref="A39:U39"/>
     <mergeCell ref="A4:U4"/>
+    <mergeCell ref="A5:U5"/>
+    <mergeCell ref="A15:U15"/>
+    <mergeCell ref="A16:U16"/>
+    <mergeCell ref="A17:U17"/>
+    <mergeCell ref="A20:U20"/>
+    <mergeCell ref="A8:U8"/>
+    <mergeCell ref="A11:U11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>